<commit_message>
Add private api platform get saved deals by user
</commit_message>
<xml_diff>
--- a/rendu_projet/Rendu-Projet-Complet-BRUNEL-LEMTAYER.xlsx
+++ b/rendu_projet/Rendu-Projet-Complet-BRUNEL-LEMTAYER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brufl\projets\projets_lp\php\dealabs\rendu_projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D45BDAE-4BE8-43ED-ABBC-56E50CA42F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A292FC8A-D285-43DD-8FA4-285E38B90DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A58EC350-CF33-BC4F-BC06-897311A7761F}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{A58EC350-CF33-BC4F-BC06-897311A7761F}"/>
   </bookViews>
   <sheets>
     <sheet name="Partie 1" sheetId="1" r:id="rId1"/>
@@ -146,10 +146,10 @@
 Pour ce qui est du cron pour l'envoi de mail tous les jours, il n'est pas mis en place mais la command et le service auquel la command doit faire appel sont prêts</t>
   </si>
   <si>
-    <t>À finir</t>
-  </si>
-  <si>
     <t>Dealabs - Partie 2</t>
+  </si>
+  <si>
+    <t>Non fini - manque la sécurité (documentation API PLATFORM ne fonctionne pas) avec JWT (lexik)</t>
   </si>
 </sst>
 </file>
@@ -235,11 +235,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -689,20 +689,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
     </row>
     <row r="3" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -897,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995777F5-5494-3840-AC9A-36EDD3A31EBD}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -908,20 +908,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="A1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
     </row>
     <row r="3" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -1010,7 +1010,7 @@
       <c r="B14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1046,7 +1046,7 @@
         <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>